<commit_message>
+completa implementacion de consulta web +adiciona filtro de monedas en consulta a base de datos en Cambiador.java +mejora ActualizaTC parausar iterador y buscar monedas que el usuario ya habia seleccionado par visualizar +creacion de la actividad configurar.java
</commit_message>
<xml_diff>
--- a/Analisis.xlsx
+++ b/Analisis.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16035" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Diagrama Flujo Activ Principal" sheetId="1" r:id="rId1"/>
     <sheet name="Botones Activ Principal" sheetId="2" r:id="rId2"/>
+    <sheet name="Diagrama Flujo Activ Config" sheetId="3" r:id="rId3"/>
+    <sheet name="Botones Activ Config" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -2156,6 +2158,2607 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectángulo redondeado 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="209550" y="190501"/>
+          <a:ext cx="2028825" cy="4838700"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-PE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CuadroTexto 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="323850" y="5219700"/>
+          <a:ext cx="1685925" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1100"/>
+            <a:t>Actividad Configuracion</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>261939</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo redondeado 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2547939" y="252413"/>
+          <a:ext cx="1135061" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>Activity</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>(On Create)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>261939</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectángulo redondeado 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2547939" y="952500"/>
+          <a:ext cx="1135061" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>Activity</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>(On Start)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>67470</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>67470</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Conector recto de flecha 5"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3115470" y="681038"/>
+          <a:ext cx="0" cy="271462"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>450851</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>484188</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectángulo redondeado 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5784851" y="2300288"/>
+          <a:ext cx="1557337" cy="428624"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>Borra elementos</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>163513</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectángulo redondeado 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3819526" y="1619250"/>
+          <a:ext cx="1677987" cy="428624"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>Lee tipos de cambio (todos)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>(base de datos)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>163513</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectángulo redondeado 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3819526" y="2300288"/>
+          <a:ext cx="1677987" cy="428624"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>Actualiza</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900" baseline="0"/>
+            <a:t> lista</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-PE" sz="900"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>58738</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>484187</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106362</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectángulo redondeado 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7308850" y="2916238"/>
+          <a:ext cx="1557337" cy="428624"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>Adiciona tipos de cambio</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>249238</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Conector recto de flecha 15"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="23" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3683000" y="1166813"/>
+          <a:ext cx="376238" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>86520</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>86520</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Conector recto de flecha 16"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="2"/>
+          <a:endCxn id="11" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4658520" y="1381125"/>
+          <a:ext cx="0" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>86520</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>86520</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Conector recto de flecha 18"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="2"/>
+          <a:endCxn id="12" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4658520" y="2047874"/>
+          <a:ext cx="0" cy="252414"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>163513</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>450851</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Conector recto de flecha 19"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="3"/>
+          <a:endCxn id="9" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5497513" y="2514600"/>
+          <a:ext cx="287338" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>467519</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>467520</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>58738</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Conector recto de flecha 20"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="2"/>
+          <a:endCxn id="13" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6563519" y="2728912"/>
+          <a:ext cx="1" cy="187326"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>249238</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>685801</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Rectángulo redondeado 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4059238" y="952500"/>
+          <a:ext cx="1198563" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>Librería WebService</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>(On Response)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Heptágono 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3000375" y="2270125"/>
+          <a:ext cx="381000" cy="365125"/>
+        </a:xfrm>
+        <a:prstGeom prst="heptagon">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1100"/>
+            <a:t>A</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333376</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28439</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Conector recto de flecha 35"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="35" idx="1"/>
+          <a:endCxn id="12" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3381376" y="2504939"/>
+          <a:ext cx="438150" cy="9661"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectángulo redondeado 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="361950" y="209550"/>
+          <a:ext cx="2028825" cy="4838700"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-PE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CuadroTexto 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="476250" y="5238749"/>
+          <a:ext cx="1685925" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1100"/>
+            <a:t>Actividad principal</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>246063</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>193675</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo redondeado 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2532063" y="2190750"/>
+          <a:ext cx="1471612" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>Check Box</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>(On change)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>193675</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>111124</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>456406</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Conector recto de flecha 4"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="9" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4003675" y="2397124"/>
+          <a:ext cx="262731" cy="7939"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>134938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>349251</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectángulo redondeado 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="904876" y="706438"/>
+          <a:ext cx="968375" cy="555625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1100"/>
+            <a:t>ACTUALIZAR TIPO CAMBIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>246064</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>193676</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectángulo redondeado 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2532064" y="690563"/>
+          <a:ext cx="1471612" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>Botón Actualizar</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>(On click)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>456406</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>87312</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>345282</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>134936</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectángulo redondeado 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4266406" y="2182812"/>
+          <a:ext cx="1412876" cy="428624"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>Identifica Tipo Cambio (Seleccionado/presionado)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>193676</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>460375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>150811</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Conector recto de flecha 10"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="3"/>
+          <a:endCxn id="34" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4003676" y="904876"/>
+          <a:ext cx="266699" cy="7935"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>448468</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>150813</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>337344</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>7937</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectángulo redondeado 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4258468" y="2817813"/>
+          <a:ext cx="1412876" cy="428624"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>Actualiza Registro </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>(Base Datos)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>392906</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>134936</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400844</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>150813</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Conector recto de flecha 13"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="2"/>
+          <a:endCxn id="12" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4964906" y="2611436"/>
+          <a:ext cx="7938" cy="206377"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>158751</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>730250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="Grupo 26"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="523875" y="1682751"/>
+          <a:ext cx="1730375" cy="2333624"/>
+          <a:chOff x="603250" y="1658939"/>
+          <a:chExt cx="1730375" cy="2333624"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Rectángulo redondeado 5"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="603250" y="1658939"/>
+            <a:ext cx="1730375" cy="2333624"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 8712"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="es-PE" sz="1100"/>
+              <a:t>LISTA</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="Rectángulo 15"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="722313" y="2214563"/>
+            <a:ext cx="277812" cy="301625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="es-PE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="CuadroTexto 16"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1087437" y="2238375"/>
+            <a:ext cx="730250" cy="254000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:endParaRPr lang="es-PE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="Rectángulo 17"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="722313" y="2555876"/>
+            <a:ext cx="277812" cy="301625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="es-PE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="CuadroTexto 18"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1087437" y="2579688"/>
+            <a:ext cx="730250" cy="254000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:endParaRPr lang="es-PE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="Rectángulo 19"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="722313" y="2928938"/>
+            <a:ext cx="277812" cy="301625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="es-PE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="21" name="CuadroTexto 20"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1087437" y="2952750"/>
+            <a:ext cx="730250" cy="254000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:endParaRPr lang="es-PE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="22" name="Rectángulo 21"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1984375" y="2182813"/>
+            <a:ext cx="277812" cy="1476374"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="es-PE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="Triángulo isósceles 22"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1988344" y="1936750"/>
+            <a:ext cx="269875" cy="214313"/>
+          </a:xfrm>
+          <a:prstGeom prst="triangle">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="es-PE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="Triángulo isósceles 23"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="1988344" y="3690937"/>
+            <a:ext cx="269875" cy="214313"/>
+          </a:xfrm>
+          <a:prstGeom prst="triangle">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="es-PE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="Rectángulo 24"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="738188" y="3294063"/>
+            <a:ext cx="277812" cy="301625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="es-PE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="26" name="CuadroTexto 25"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1103312" y="3317875"/>
+            <a:ext cx="730250" cy="254000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:endParaRPr lang="es-PE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>7937</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Multiplicar 28"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="698500" y="2293937"/>
+          <a:ext cx="182562" cy="246063"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-PE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Multiplicar 29"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="698500" y="3000375"/>
+          <a:ext cx="182562" cy="246063"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-PE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>460375</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>126999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>365124</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>174623</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Rectángulo redondeado 33"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4270375" y="698499"/>
+          <a:ext cx="1428749" cy="428624"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>Lee tipo de cambio</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>(web service)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>601663</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>176211</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Rectángulo redondeado 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5935663" y="1271587"/>
+          <a:ext cx="1677987" cy="428624"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>Actualiza tipos de cambio (todos)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>(base de datos)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>678657</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>174624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>678657</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Conector recto de flecha 35"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="37" idx="2"/>
+          <a:endCxn id="35" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6774657" y="1127124"/>
+          <a:ext cx="0" cy="144463"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>79375</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>126999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>515938</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>174624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="Rectángulo redondeado 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6175375" y="698499"/>
+          <a:ext cx="1198563" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>Librería WebService</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1000"/>
+            <a:t>(On Response)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>365124</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>150811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>79375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>150812</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Conector recto de flecha 37"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="34" idx="3"/>
+          <a:endCxn id="37" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5699124" y="912811"/>
+          <a:ext cx="476251" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>103188</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>87313</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Heptágono 50"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8064500" y="1246188"/>
+          <a:ext cx="381000" cy="365125"/>
+        </a:xfrm>
+        <a:prstGeom prst="heptagon">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="1100"/>
+            <a:t>A</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>147502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>444499</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Conector recto de flecha 51"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="35" idx="3"/>
+          <a:endCxn id="51" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7613650" y="1481002"/>
+          <a:ext cx="450849" cy="4897"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>103187</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>436562</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="CuadroTexto 55"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7723187" y="1682750"/>
+          <a:ext cx="1095375" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-PE" sz="900"/>
+            <a:t>(ACTUALIZA LISTA)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2426,7 +5029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
@@ -2450,4 +5053,34 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
+conclusion de actividad configurar +aplicacion completa +documentacion completa
</commit_message>
<xml_diff>
--- a/Analisis.xlsx
+++ b/Analisis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16035" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16035" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Diagrama Flujo Activ Principal" sheetId="1" r:id="rId1"/>
@@ -2461,15 +2461,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>450851</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:colOff>681039</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>484188</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>714376</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2478,7 +2478,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5784851" y="2300288"/>
+          <a:off x="6015039" y="1657351"/>
           <a:ext cx="1557337" cy="428624"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -2515,16 +2515,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>163513</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:colOff>715964</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7934</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>690563</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>55558</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2533,8 +2533,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3819526" y="1619250"/>
-          <a:ext cx="1677987" cy="428624"/>
+          <a:off x="6049964" y="960434"/>
+          <a:ext cx="1498599" cy="428624"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2578,15 +2578,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:colOff>319089</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>6351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>163513</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>473076</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2595,7 +2595,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3819526" y="2300288"/>
+          <a:off x="4129089" y="958851"/>
           <a:ext cx="1677987" cy="428624"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -2638,15 +2638,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>58738</xdr:rowOff>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177801</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>484187</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>106362</xdr:rowOff>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2655,7 +2655,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7308850" y="2916238"/>
+          <a:off x="6015038" y="2273301"/>
           <a:ext cx="1557337" cy="428624"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -2699,22 +2699,22 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>249238</xdr:colOff>
+      <xdr:colOff>319089</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>23813</xdr:rowOff>
+      <xdr:rowOff>30163</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="16" name="Conector recto de flecha 15"/>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="5" idx="3"/>
-          <a:endCxn id="23" idx="1"/>
+          <a:endCxn id="12" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3683000" y="1166813"/>
-          <a:ext cx="376238" cy="0"/>
+          <a:ext cx="446089" cy="6350"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2742,79 +2742,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>86520</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>697708</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>86520</xdr:colOff>
+      <xdr:rowOff>55558</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>703264</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Conector recto de flecha 16"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="23" idx="2"/>
-          <a:endCxn id="11" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4658520" y="1381125"/>
-          <a:ext cx="0" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>86520</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>86520</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="19" name="Conector recto de flecha 18"/>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="11" idx="2"/>
-          <a:endCxn id="12" idx="0"/>
+          <a:endCxn id="9" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4658520" y="2047874"/>
-          <a:ext cx="0" cy="252414"/>
+        <a:xfrm flipH="1">
+          <a:off x="6793708" y="1389058"/>
+          <a:ext cx="5556" cy="268293"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2843,28 +2793,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>163513</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>473076</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>30163</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>450851</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>715964</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>31746</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="20" name="Conector recto de flecha 19"/>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="12" idx="3"/>
-          <a:endCxn id="9" idx="1"/>
+          <a:endCxn id="11" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5497513" y="2514600"/>
-          <a:ext cx="287338" cy="0"/>
+          <a:off x="5807076" y="1173163"/>
+          <a:ext cx="242888" cy="1583"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2893,15 +2843,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>467519</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>697707</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>467520</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>58738</xdr:rowOff>
+      <xdr:colOff>697708</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177801</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2913,7 +2863,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6563519" y="2728912"/>
+          <a:off x="6793707" y="2085975"/>
           <a:ext cx="1" cy="187326"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2942,79 +2892,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>249238</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>685801</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Rectángulo redondeado 22"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4059238" y="952500"/>
-          <a:ext cx="1198563" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1000"/>
-            <a:t>Librería WebService</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1000"/>
-            <a:t>(On Response)</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>39688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>174625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:rowOff>23813</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3023,7 +2910,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3000375" y="2270125"/>
+          <a:off x="3071812" y="1754188"/>
           <a:ext cx="381000" cy="365125"/>
         </a:xfrm>
         <a:prstGeom prst="heptagon">
@@ -3061,28 +2948,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>333376</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>28439</xdr:rowOff>
+      <xdr:colOff>367081</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>30163</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>319089</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>112006</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="36" name="Conector recto de flecha 35"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="35" idx="1"/>
+          <a:stCxn id="35" idx="0"/>
           <a:endCxn id="12" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3381376" y="2504939"/>
-          <a:ext cx="438150" cy="9661"/>
+        <a:xfrm flipV="1">
+          <a:off x="3415081" y="1173163"/>
+          <a:ext cx="714008" cy="653343"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5059,8 +4946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5074,8 +4961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>